<commit_message>
product : html/css, fonctions terminés
</commit_message>
<xml_diff>
--- a/spécifications/test unitaire.xlsx
+++ b/spécifications/test unitaire.xlsx
@@ -16,32 +16,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>fichier</t>
   </si>
   <si>
-    <t>product,js</t>
-  </si>
-  <si>
-    <t>17 a 23</t>
-  </si>
-  <si>
     <t>ligne</t>
   </si>
   <si>
-    <t>le json du produit correspondant à l'id</t>
-  </si>
-  <si>
     <t>résultat attendu</t>
   </si>
   <si>
-    <t>tester avec identifiant</t>
-  </si>
-  <si>
-    <t>le produit retourné ne correspond pas à l'id</t>
-  </si>
-  <si>
     <t>comment vérifier</t>
   </si>
   <si>
@@ -66,26 +51,130 @@
     <t>la base de données peut être vide</t>
   </si>
   <si>
-    <t>affichage des objets json</t>
-  </si>
-  <si>
-    <t>téléchargement des objets json</t>
-  </si>
-  <si>
     <t>tester une variable  qui contient des objets json avec les propriétés nécessaires (id, url des images, nom, description)</t>
+  </si>
+  <si>
+    <t>product.js</t>
+  </si>
+  <si>
+    <t>28 à 35</t>
+  </si>
+  <si>
+    <t>tester une liste de couleurs et voir si les options apparaissent bien dans un select créé pour le test</t>
+  </si>
+  <si>
+    <t>la liste de couleurs est vide, le select n'existe pas</t>
+  </si>
+  <si>
+    <t>nom de la fonction</t>
+  </si>
+  <si>
+    <t>DisplayDownloadProducts</t>
+  </si>
+  <si>
+    <t>downloadProducts</t>
+  </si>
+  <si>
+    <t>AddSelectOption</t>
+  </si>
+  <si>
+    <t>38 à 41</t>
+  </si>
+  <si>
+    <r>
+      <t>AddToLocalStorage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>affichage des objets json téléchargés</t>
+  </si>
+  <si>
+    <t>téléchargement des objets json à afficher</t>
+  </si>
+  <si>
+    <t>ajout des options de couleurs de personnalisation de l'objet json affiché</t>
+  </si>
+  <si>
+    <t>ajout au localStorage du tableau contenant l'ensemble des articles à mettre dans le panier en l'associant à la clé produit</t>
+  </si>
+  <si>
+    <t>tester un tableau contenant des objets</t>
+  </si>
+  <si>
+    <t>le tableau peut être vide, la clé n'existe pas dans le localStorage</t>
+  </si>
+  <si>
+    <t>44 à 64</t>
+  </si>
+  <si>
+    <t>AddProductsToCart</t>
+  </si>
+  <si>
+    <t>tester une liste de produits</t>
+  </si>
+  <si>
+    <t>ajout de la liste des produits dans le panier avec l'option d'ajouter une quantité à un produit</t>
+  </si>
+  <si>
+    <t>la liste de produits est vide, l'id du produit ne correspond pas à aucun id présent dans la liste</t>
+  </si>
+  <si>
+    <t>67 à 130</t>
+  </si>
+  <si>
+    <t>DisplayDownloadedProduct</t>
+  </si>
+  <si>
+    <t>tester un objet json</t>
+  </si>
+  <si>
+    <t>les propriétés de l'objet ne sont pas celles attendues</t>
+  </si>
+  <si>
+    <t>133 à 144</t>
+  </si>
+  <si>
+    <t>DownloadProductById</t>
+  </si>
+  <si>
+    <t>téléchargement de l'objet json</t>
+  </si>
+  <si>
+    <t>affichage de l'objet json</t>
+  </si>
+  <si>
+    <t>tester avec un url et un id</t>
+  </si>
+  <si>
+    <t>l'url de l'api ne répond pas, l'id n'existe pas dans la base de données</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -405,89 +494,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="111" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="5" max="5" width="111" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ajout evenement unload à cart.js, modification de la barre de navigation
</commit_message>
<xml_diff>
--- a/spécifications/test unitaire.xlsx
+++ b/spécifications/test unitaire.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
   <si>
     <t>fichier</t>
   </si>
@@ -161,9 +161,6 @@
     <t>cart.js</t>
   </si>
   <si>
-    <t>31 à 63</t>
-  </si>
-  <si>
     <t>DisplayForm</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>l'emplacement n'existe pas</t>
   </si>
   <si>
-    <t>69 à 104</t>
-  </si>
-  <si>
     <t>SendContactProductsId</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
     <t>le serveur ne répond pas, les noms des propriétés de l'objet ne correspondent aux noms attendus par le serveur, les id n'existent pas dans la base des données produits,  la page de redirection n'existe pas</t>
   </si>
   <si>
-    <t>108 à 207</t>
-  </si>
-  <si>
     <t>CollectContactProductsId</t>
   </si>
   <si>
@@ -206,9 +197,6 @@
     <t>la liste de produits est vide, les valeurs des contrôles ne correspondent pas aux normes attendus</t>
   </si>
   <si>
-    <t>210 à 286</t>
-  </si>
-  <si>
     <t>DisplayProductsLocalStorage</t>
   </si>
   <si>
@@ -221,18 +209,12 @@
     <t>la liste de produit soit vide, l'emplacement n'existe pas sur la page panier</t>
   </si>
   <si>
-    <t>306 à 330</t>
-  </si>
-  <si>
     <t>DecreaseProductQuantity</t>
   </si>
   <si>
     <t>diminuer la quantité d'un article</t>
   </si>
   <si>
-    <t>340 à 360</t>
-  </si>
-  <si>
     <t>IncreaseProductQuantity</t>
   </si>
   <si>
@@ -242,9 +224,6 @@
     <t>la liste de produits peut être vide, les boutons n'existent pas, l'id du produit ne se trouve pas dans  la clé de stockage localStorage des produits, la clé de stockage produit n'existe pas</t>
   </si>
   <si>
-    <t>370 à 389</t>
-  </si>
-  <si>
     <t>DeleteProduct</t>
   </si>
   <si>
@@ -291,6 +270,45 @@
   </si>
   <si>
     <t>la page de redirection n'existe pas, les clés mentionnées dans la fonction ne sont pas présentes dans le localStorage</t>
+  </si>
+  <si>
+    <t>34 à 66</t>
+  </si>
+  <si>
+    <t>72 à 106</t>
+  </si>
+  <si>
+    <t>110 à 209</t>
+  </si>
+  <si>
+    <t>212 à 286</t>
+  </si>
+  <si>
+    <t>card.js</t>
+  </si>
+  <si>
+    <t>301 à 380</t>
+  </si>
+  <si>
+    <t>handleButtonClick</t>
+  </si>
+  <si>
+    <t>modifier la quantité d'un article du panier en mettant à jour la quantité totale d'articles et le montant total de la commande</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>la liste de produits soit vide, que l'id du produit ne soit pas présent dans la liste du panier, la clé associée à au produit ne soit pas présente dans le localStorage, l'emplacement de l'affichage du montant de la commande et de la quantité des articles n'existent pas, le rechargement de la page ne soit pas effectif</t>
+  </si>
+  <si>
+    <t>390 à 396</t>
+  </si>
+  <si>
+    <t>406 à 412</t>
+  </si>
+  <si>
+    <t>422 à 429</t>
   </si>
 </sst>
 </file>
@@ -634,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -650,7 +668,7 @@
     <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -670,7 +688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60">
+    <row r="2" spans="1:7" ht="60">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -690,7 +708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -710,7 +728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45">
+    <row r="4" spans="1:7" ht="45">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -730,7 +748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45">
+    <row r="5" spans="1:7" ht="45">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -750,7 +768,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45">
+    <row r="6" spans="1:7" ht="45">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -770,7 +788,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -790,7 +808,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30">
+    <row r="8" spans="1:7" ht="30">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -810,184 +828,207 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="90">
+    </row>
+    <row r="10" spans="1:7" ht="90">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="60">
+    </row>
+    <row r="11" spans="1:7" ht="60">
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="60">
+    </row>
+    <row r="12" spans="1:7" ht="60">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="90">
+    </row>
+    <row r="13" spans="1:7" ht="150">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="90">
+        <v>90</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="90">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="90">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="90">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="90">
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="75">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="60">
+      <c r="A18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="75">
-      <c r="A16" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="60">
-      <c r="A17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modif du plan de test
</commit_message>
<xml_diff>
--- a/spécifications/test unitaire.xlsx
+++ b/spécifications/test unitaire.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="98">
   <si>
     <t>fichier</t>
   </si>
@@ -266,9 +266,6 @@
     <t>la page de redirection n'existe pas, les clés mentionnées dans la fonction ne sont pas présentes dans le localStorage</t>
   </si>
   <si>
-    <t>card.js</t>
-  </si>
-  <si>
     <t>handleButtonClick</t>
   </si>
   <si>
@@ -305,25 +302,25 @@
     <t>les variables regex ne sont pas déclarées, les valeurs ne remplissent pas les conditions du regex</t>
   </si>
   <si>
-    <t>128 à 176</t>
-  </si>
-  <si>
-    <t>179 à 255</t>
-  </si>
-  <si>
     <t>modifier la quantité d'un article du panier</t>
   </si>
   <si>
-    <t>270 à 431</t>
-  </si>
-  <si>
-    <t>441 à 447</t>
-  </si>
-  <si>
-    <t>457 à 463</t>
-  </si>
-  <si>
-    <t>473 à 480</t>
+    <t>128 à 189</t>
+  </si>
+  <si>
+    <t>192 à 268</t>
+  </si>
+  <si>
+    <t>283 à 444</t>
+  </si>
+  <si>
+    <t>454 à 460</t>
+  </si>
+  <si>
+    <t>470 à 476</t>
+  </si>
+  <si>
+    <t>486 à 493</t>
   </si>
 </sst>
 </file>
@@ -669,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -808,7 +805,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>33</v>
@@ -828,7 +825,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>36</v>
@@ -848,7 +845,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -868,7 +865,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>46</v>
@@ -888,19 +885,19 @@
         <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60">
@@ -945,25 +942,25 @@
     </row>
     <row r="14" spans="1:7" ht="150">
       <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90">
@@ -971,7 +968,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>58</v>
@@ -991,7 +988,7 @@
         <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>60</v>
@@ -1011,7 +1008,7 @@
         <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
tests unitaires : mise à jour des valeurs des lignes des fonctions
</commit_message>
<xml_diff>
--- a/spécifications/test unitaire.xlsx
+++ b/spécifications/test unitaire.xlsx
@@ -275,21 +275,6 @@
     <t>la liste de produits soit vide, que l'id du produit ne soit pas présent dans la liste du panier, la clé associée à au produit ne soit pas présente dans le localStorage, l'emplacement de l'affichage du montant de la commande et de la quantité des articles n'existent pas, le rechargement de la page ne soit pas effectif</t>
   </si>
   <si>
-    <t>67 à 136</t>
-  </si>
-  <si>
-    <t>139 à 150</t>
-  </si>
-  <si>
-    <t>42 à 74</t>
-  </si>
-  <si>
-    <t>80 à 114</t>
-  </si>
-  <si>
-    <t>119 à 125</t>
-  </si>
-  <si>
     <t>ControlValues</t>
   </si>
   <si>
@@ -305,22 +290,37 @@
     <t>modifier la quantité d'un article du panier</t>
   </si>
   <si>
-    <t>128 à 189</t>
-  </si>
-  <si>
-    <t>192 à 268</t>
-  </si>
-  <si>
-    <t>283 à 444</t>
-  </si>
-  <si>
-    <t>454 à 460</t>
-  </si>
-  <si>
-    <t>470 à 476</t>
-  </si>
-  <si>
-    <t>486 à 493</t>
+    <t>43 à 75</t>
+  </si>
+  <si>
+    <t>81 à 112</t>
+  </si>
+  <si>
+    <t>117 à 123</t>
+  </si>
+  <si>
+    <t>126 à 186</t>
+  </si>
+  <si>
+    <t>189 à 265</t>
+  </si>
+  <si>
+    <t>280 à 398</t>
+  </si>
+  <si>
+    <t>408 à 414</t>
+  </si>
+  <si>
+    <t>424 à 430</t>
+  </si>
+  <si>
+    <t>440 à 447</t>
+  </si>
+  <si>
+    <t>67 à 137</t>
+  </si>
+  <si>
+    <t>140 à 151</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -805,7 +805,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>33</v>
@@ -825,7 +825,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>36</v>
@@ -845,7 +845,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
@@ -865,7 +865,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>46</v>
@@ -885,19 +885,19 @@
         <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60">
@@ -905,7 +905,7 @@
         <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>49</v>
@@ -925,7 +925,7 @@
         <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>54</v>
@@ -945,13 +945,13 @@
         <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>34</v>
@@ -968,7 +968,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>58</v>
@@ -988,7 +988,7 @@
         <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>60</v>
@@ -1008,7 +1008,7 @@
         <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>63</v>

</xml_diff>